<commit_message>
fix bug related to INCLUDE_RESOURCE_RECOVERY
</commit_message>
<xml_diff>
--- a/dmsan/comparison/scores/percentiles.xlsx
+++ b/dmsan/comparison/scores/percentiles.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO12"/>
+  <dimension ref="A1:AO16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,79 +793,79 @@
         <v>67.35540000000003</v>
       </c>
       <c r="Q5" t="n">
-        <v>8.980638249763535</v>
+        <v>8.087738042848772</v>
       </c>
       <c r="R5" t="n">
-        <v>10.35778954650501</v>
+        <v>10.57913364387923</v>
       </c>
       <c r="S5" t="n">
-        <v>13.79391689805261</v>
+        <v>12.82304730224299</v>
       </c>
       <c r="T5" t="n">
-        <v>16.9761790602927</v>
+        <v>16.83036879736425</v>
       </c>
       <c r="U5" t="n">
-        <v>23.3685805030534</v>
+        <v>26.11906035821446</v>
       </c>
       <c r="V5" t="n">
-        <v>9.095560293128997</v>
+        <v>9.917023342668969</v>
       </c>
       <c r="W5" t="n">
-        <v>20.81760089846793</v>
+        <v>22.74825595050666</v>
       </c>
       <c r="X5" t="n">
-        <v>33.89096390541366</v>
+        <v>32.88234543074218</v>
       </c>
       <c r="Y5" t="n">
-        <v>45.10166889313972</v>
+        <v>43.13465367526462</v>
       </c>
       <c r="Z5" t="n">
-        <v>53.75399956318864</v>
+        <v>54.39241914938081</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.04074527061530655</v>
+        <v>-0.04180757251822971</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.02409811360311736</v>
+        <v>-0.01527188243997782</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.0005614905614153391</v>
+        <v>0.002877788385915267</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.05460619539099006</v>
+        <v>0.04080733381307131</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.1256852273545591</v>
+        <v>0.1135684602602405</v>
       </c>
       <c r="AF5" t="n">
-        <v>2.146520314084465</v>
+        <v>2.934830423197214</v>
       </c>
       <c r="AG5" t="n">
-        <v>5.473638394732986</v>
+        <v>6.185422383932008</v>
       </c>
       <c r="AH5" t="n">
-        <v>9.255281661951658</v>
+        <v>9.577959060736129</v>
       </c>
       <c r="AI5" t="n">
-        <v>12.40408772451357</v>
+        <v>13.57968370710677</v>
       </c>
       <c r="AJ5" t="n">
-        <v>16.82310267875612</v>
+        <v>17.25435862260653</v>
       </c>
       <c r="AK5" t="n">
-        <v>-0.4115263679171393</v>
+        <v>-0.4580102289340602</v>
       </c>
       <c r="AL5" t="n">
-        <v>-0.2695682049203774</v>
+        <v>-0.266406022945469</v>
       </c>
       <c r="AM5" t="n">
-        <v>-0.1425549358904353</v>
+        <v>-0.1594714392347532</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.03315272594329302</v>
+        <v>-0.002062340154018127</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.2960487410609615</v>
+        <v>0.2888533005204561</v>
       </c>
     </row>
     <row r="6">
@@ -920,79 +920,79 @@
         <v>67.35540000000003</v>
       </c>
       <c r="Q6" t="n">
-        <v>6.418765001650569</v>
+        <v>6.224291864630196</v>
       </c>
       <c r="R6" t="n">
-        <v>8.148051108366829</v>
+        <v>7.449522885849793</v>
       </c>
       <c r="S6" t="n">
-        <v>9.563903639785046</v>
+        <v>8.624643728619951</v>
       </c>
       <c r="T6" t="n">
-        <v>10.9596631137221</v>
+        <v>11.58662664154168</v>
       </c>
       <c r="U6" t="n">
-        <v>18.06244735444609</v>
+        <v>18.35767669504722</v>
       </c>
       <c r="V6" t="n">
-        <v>11.69323191388979</v>
+        <v>10.59816265013006</v>
       </c>
       <c r="W6" t="n">
-        <v>16.17319728442209</v>
+        <v>20.06790637427611</v>
       </c>
       <c r="X6" t="n">
-        <v>24.43822152040469</v>
+        <v>28.95303335199505</v>
       </c>
       <c r="Y6" t="n">
-        <v>45.40115032992063</v>
+        <v>40.1706473959436</v>
       </c>
       <c r="Z6" t="n">
-        <v>56.7172002221028</v>
+        <v>55.33685177868236</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.05601794907819488</v>
+        <v>-0.04893517594354576</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.0233736555017621</v>
+        <v>-0.02410529891983469</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.01190404848597431</v>
+        <v>-0.01181919093590878</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.01096480495465373</v>
+        <v>0.01386879817719226</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.07143147133562414</v>
+        <v>0.07814567242497604</v>
       </c>
       <c r="AF6" t="n">
-        <v>3.852497739400552</v>
+        <v>2.444010673860972</v>
       </c>
       <c r="AG6" t="n">
-        <v>5.336532327332533</v>
+        <v>5.778751638759922</v>
       </c>
       <c r="AH6" t="n">
-        <v>7.416243929174417</v>
+        <v>8.770317349111558</v>
       </c>
       <c r="AI6" t="n">
-        <v>14.29151381917629</v>
+        <v>13.53762651639766</v>
       </c>
       <c r="AJ6" t="n">
-        <v>17.96910481545113</v>
+        <v>19.79993679210718</v>
       </c>
       <c r="AK6" t="n">
-        <v>-0.501059987585638</v>
+        <v>-0.4679744404066874</v>
       </c>
       <c r="AL6" t="n">
-        <v>-0.2917911167730826</v>
+        <v>-0.2831482258531127</v>
       </c>
       <c r="AM6" t="n">
-        <v>-0.2375883247092201</v>
+        <v>-0.1948375107910687</v>
       </c>
       <c r="AN6" t="n">
-        <v>-0.0929823960818367</v>
+        <v>-0.09945419367116916</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.09564433011910266</v>
+        <v>0.1651259964220518</v>
       </c>
     </row>
     <row r="7">
@@ -1047,79 +1047,79 @@
         <v>72.52000000000002</v>
       </c>
       <c r="Q7" t="n">
-        <v>18.256562808281</v>
+        <v>16.34906875584214</v>
       </c>
       <c r="R7" t="n">
-        <v>20.60410385538651</v>
+        <v>19.77607753250028</v>
       </c>
       <c r="S7" t="n">
-        <v>24.55511594817131</v>
+        <v>22.24014516877218</v>
       </c>
       <c r="T7" t="n">
-        <v>31.31570642751312</v>
+        <v>27.1643867009142</v>
       </c>
       <c r="U7" t="n">
-        <v>38.25240393601572</v>
+        <v>37.26085037010203</v>
       </c>
       <c r="V7" t="n">
-        <v>-2.066594520867296</v>
+        <v>-0.9506964077571354</v>
       </c>
       <c r="W7" t="n">
-        <v>2.492027703553028</v>
+        <v>2.076659253809259</v>
       </c>
       <c r="X7" t="n">
-        <v>5.65904261222227</v>
+        <v>7.832698690676954</v>
       </c>
       <c r="Y7" t="n">
-        <v>16.59439946659898</v>
+        <v>15.96471980147177</v>
       </c>
       <c r="Z7" t="n">
-        <v>48.45145115456291</v>
+        <v>33.8385915075303</v>
       </c>
       <c r="AA7" t="n">
-        <v>-0.03265107850479199</v>
+        <v>0.003552671470622268</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.01661897864741172</v>
+        <v>0.02715662677184152</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.04012625475845869</v>
+        <v>0.05237068693167696</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.09330355429311438</v>
+        <v>0.1100801699650429</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.2418550122817007</v>
+        <v>0.1983531566657925</v>
       </c>
       <c r="AF7" t="n">
-        <v>-0.9182518162519282</v>
+        <v>-0.4072922120698385</v>
       </c>
       <c r="AG7" t="n">
-        <v>-0.08129699318794044</v>
+        <v>-0.03217729677168402</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.3762986548320829</v>
+        <v>0.486368650193742</v>
       </c>
       <c r="AI7" t="n">
-        <v>1.254640454913893</v>
+        <v>1.099598202143781</v>
       </c>
       <c r="AJ7" t="n">
-        <v>2.658522287026424</v>
+        <v>2.064958864197429</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.4190525367066393</v>
+        <v>0.6401336667215977</v>
       </c>
       <c r="AL7" t="n">
-        <v>1.045074789420438</v>
+        <v>1.10773644644204</v>
       </c>
       <c r="AM7" t="n">
-        <v>1.310126132852843</v>
+        <v>1.450723923531111</v>
       </c>
       <c r="AN7" t="n">
-        <v>2.018403945785684</v>
+        <v>1.930932416666497</v>
       </c>
       <c r="AO7" t="n">
-        <v>2.840665463028808</v>
+        <v>2.820947623399217</v>
       </c>
     </row>
     <row r="8">
@@ -1174,587 +1174,1095 @@
         <v>72.52000000000002</v>
       </c>
       <c r="Q8" t="n">
-        <v>16.96920505514503</v>
+        <v>13.68571000637046</v>
       </c>
       <c r="R8" t="n">
-        <v>19.25752144636215</v>
+        <v>16.12316520108278</v>
       </c>
       <c r="S8" t="n">
-        <v>20.26295133869913</v>
+        <v>17.86128185422622</v>
       </c>
       <c r="T8" t="n">
-        <v>22.48874921790248</v>
+        <v>20.57906164876427</v>
       </c>
       <c r="U8" t="n">
-        <v>30.44425085016551</v>
+        <v>28.40569692720842</v>
       </c>
       <c r="V8" t="n">
-        <v>-3.62881138001699</v>
+        <v>-2.967103172487918</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.5030321554222578</v>
+        <v>0.04174067583269786</v>
       </c>
       <c r="X8" t="n">
-        <v>3.554912204130554</v>
+        <v>3.398100216710654</v>
       </c>
       <c r="Y8" t="n">
-        <v>9.445047434867714</v>
+        <v>7.757504844770218</v>
       </c>
       <c r="Z8" t="n">
-        <v>26.89039832868938</v>
+        <v>27.20532725576395</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.009149717879399619</v>
+        <v>-0.01982853263668472</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.01523530316863492</v>
+        <v>0.01689333511176202</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.03402019533628004</v>
+        <v>0.03526644436764682</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.06991047275457704</v>
+        <v>0.06385420267986985</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.147028568871975</v>
+        <v>0.1691940061099927</v>
       </c>
       <c r="AF8" t="n">
-        <v>-0.5505305289779505</v>
+        <v>-1.061799603283503</v>
       </c>
       <c r="AG8" t="n">
-        <v>-0.2214154689282009</v>
+        <v>-0.1146550674090234</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.2524691569039468</v>
+        <v>0.2791338854711863</v>
       </c>
       <c r="AI8" t="n">
-        <v>1.045345286350298</v>
+        <v>0.9476700929420968</v>
       </c>
       <c r="AJ8" t="n">
-        <v>1.76747058446496</v>
+        <v>2.010714270522354</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.6609411761478158</v>
+        <v>0.4781732959095543</v>
       </c>
       <c r="AL8" t="n">
-        <v>1.084960616671619</v>
+        <v>0.9611592357234144</v>
       </c>
       <c r="AM8" t="n">
-        <v>1.336445416306187</v>
+        <v>1.363816070698125</v>
       </c>
       <c r="AN8" t="n">
-        <v>1.612851931468903</v>
+        <v>1.842018119364146</v>
       </c>
       <c r="AO8" t="n">
-        <v>2.527916014247432</v>
+        <v>2.403114178828788</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>reB_BeijingChina</t>
+          <t>ngA_BeijingChina</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="C9" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="D9" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="E9" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="F9" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="G9" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="H9" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="I9" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="J9" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="K9" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="L9" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="M9" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="N9" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="O9" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="P9" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="Q9" t="n">
-        <v>104.6370472506634</v>
+        <v>37.99019020486618</v>
       </c>
       <c r="R9" t="n">
-        <v>123.3490342820781</v>
+        <v>42.13615427609541</v>
       </c>
       <c r="S9" t="n">
-        <v>129.342356228268</v>
+        <v>46.59542539399344</v>
       </c>
       <c r="T9" t="n">
-        <v>142.2541703641299</v>
+        <v>52.71112459478412</v>
       </c>
       <c r="U9" t="n">
-        <v>148.0720047217642</v>
+        <v>59.67508135117248</v>
       </c>
       <c r="V9" t="n">
-        <v>128.2964197808201</v>
+        <v>51.36972798548969</v>
       </c>
       <c r="W9" t="n">
-        <v>153.2663122175072</v>
+        <v>58.85069878969978</v>
       </c>
       <c r="X9" t="n">
-        <v>161.4561286615359</v>
+        <v>65.13891340906095</v>
       </c>
       <c r="Y9" t="n">
-        <v>191.0433992383494</v>
+        <v>71.93819993661398</v>
       </c>
       <c r="Z9" t="n">
-        <v>207.1446480983261</v>
+        <v>81.55077309402778</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.02388733902748548</v>
+        <v>0.06513971951825082</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.05287356958094704</v>
+        <v>0.08072203520291898</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.109407669215795</v>
+        <v>0.08971274921387161</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.1705772476546762</v>
+        <v>0.1056497654545443</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.2107123836986251</v>
+        <v>0.1163083234063428</v>
       </c>
       <c r="AF9" t="n">
-        <v>11.72027229497971</v>
+        <v>5.53956029004235</v>
       </c>
       <c r="AG9" t="n">
-        <v>19.16836853647886</v>
+        <v>7.63044056681552</v>
       </c>
       <c r="AH9" t="n">
-        <v>29.70680124621553</v>
+        <v>10.36366271443692</v>
       </c>
       <c r="AI9" t="n">
-        <v>31.63562337247774</v>
+        <v>13.39085577205625</v>
       </c>
       <c r="AJ9" t="n">
-        <v>45.31313107548866</v>
+        <v>17.01493744874055</v>
       </c>
       <c r="AK9" t="n">
-        <v>6.295089423553504</v>
+        <v>1.520631870283722</v>
       </c>
       <c r="AL9" t="n">
-        <v>7.766409610350689</v>
+        <v>1.927295687153606</v>
       </c>
       <c r="AM9" t="n">
-        <v>8.692233565490586</v>
+        <v>2.257320328405543</v>
       </c>
       <c r="AN9" t="n">
-        <v>9.814343830329163</v>
+        <v>2.995069242746312</v>
       </c>
       <c r="AO9" t="n">
-        <v>11.74879492749608</v>
+        <v>3.957390242343539</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>reB_general</t>
+          <t>ngA_general</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="C10" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="D10" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="E10" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="F10" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="G10" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="H10" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="I10" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="J10" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="K10" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="L10" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="M10" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="N10" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="O10" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="P10" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="Q10" t="n">
-        <v>87.4542744479011</v>
+        <v>34.16789777733863</v>
       </c>
       <c r="R10" t="n">
-        <v>94.45324849602542</v>
+        <v>39.12778323111338</v>
       </c>
       <c r="S10" t="n">
-        <v>111.232875084369</v>
+        <v>43.3800204347999</v>
       </c>
       <c r="T10" t="n">
-        <v>141.8466831884807</v>
+        <v>47.74062211281079</v>
       </c>
       <c r="U10" t="n">
-        <v>162.667584833289</v>
+        <v>57.98683938650231</v>
       </c>
       <c r="V10" t="n">
-        <v>106.7907182702896</v>
+        <v>50.09033148055828</v>
       </c>
       <c r="W10" t="n">
-        <v>133.8284204855148</v>
+        <v>56.87627108948169</v>
       </c>
       <c r="X10" t="n">
-        <v>177.0721096537899</v>
+        <v>64.43793923291912</v>
       </c>
       <c r="Y10" t="n">
-        <v>194.4089853878659</v>
+        <v>70.57061760980856</v>
       </c>
       <c r="Z10" t="n">
-        <v>211.6223377077261</v>
+        <v>81.32863253834125</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.03547432253356888</v>
+        <v>0.06922265942379688</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.07687836206504975</v>
+        <v>0.08240890005016921</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.1070115329552172</v>
+        <v>0.09256513104874446</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.1408886606122587</v>
+        <v>0.1082887510640705</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.2684606908755935</v>
+        <v>0.1245153377937606</v>
       </c>
       <c r="AF10" t="n">
-        <v>11.98321944277445</v>
+        <v>5.464871554217727</v>
       </c>
       <c r="AG10" t="n">
-        <v>17.69401487764711</v>
+        <v>7.761040779677252</v>
       </c>
       <c r="AH10" t="n">
-        <v>24.92349448296705</v>
+        <v>10.94055405946088</v>
       </c>
       <c r="AI10" t="n">
-        <v>39.96207368617614</v>
+        <v>13.75425071871804</v>
       </c>
       <c r="AJ10" t="n">
-        <v>45.068806347293</v>
+        <v>16.10751439430552</v>
       </c>
       <c r="AK10" t="n">
-        <v>5.711598543013153</v>
+        <v>1.530499390907173</v>
       </c>
       <c r="AL10" t="n">
-        <v>6.867250191951257</v>
+        <v>1.880742829084356</v>
       </c>
       <c r="AM10" t="n">
-        <v>8.607625291294589</v>
+        <v>2.401159818168353</v>
       </c>
       <c r="AN10" t="n">
-        <v>10.83735472449853</v>
+        <v>3.15271485946275</v>
       </c>
       <c r="AO10" t="n">
-        <v>12.35777845537645</v>
+        <v>4.054957316938868</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>reC_BeijingChina</t>
+          <t>ngB_BeijingChina</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="C11" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="D11" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="E11" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="F11" t="n">
-        <v>71.44512899511798</v>
+        <v>45.93343593776623</v>
       </c>
       <c r="G11" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="H11" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="I11" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="J11" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="K11" t="n">
-        <v>91.79485817690723</v>
+        <v>27.8335508740337</v>
       </c>
       <c r="L11" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="M11" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="N11" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="O11" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="P11" t="n">
-        <v>17.94858176907224</v>
+        <v>10.90561836300458</v>
       </c>
       <c r="Q11" t="n">
-        <v>113.6597657682182</v>
+        <v>35.51444179156612</v>
       </c>
       <c r="R11" t="n">
-        <v>133.6969358391893</v>
+        <v>39.96837952390045</v>
       </c>
       <c r="S11" t="n">
-        <v>137.6800485963101</v>
+        <v>44.06544414915727</v>
       </c>
       <c r="T11" t="n">
-        <v>151.7761610071727</v>
+        <v>50.47259923792448</v>
       </c>
       <c r="U11" t="n">
-        <v>156.4659721019006</v>
+        <v>57.43759359049805</v>
       </c>
       <c r="V11" t="n">
-        <v>84.59271284345418</v>
+        <v>64.03743615034072</v>
       </c>
       <c r="W11" t="n">
-        <v>106.8849422181489</v>
+        <v>70.26374751696395</v>
       </c>
       <c r="X11" t="n">
-        <v>120.7281944221964</v>
+        <v>77.17885575419194</v>
       </c>
       <c r="Y11" t="n">
-        <v>148.1082126667429</v>
+        <v>83.7145094474334</v>
       </c>
       <c r="Z11" t="n">
-        <v>165.9888132982445</v>
+        <v>93.43249529806047</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.1047205837191158</v>
+        <v>0.1001895218256053</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.07510474896195853</v>
+        <v>0.1182856658115652</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.03075720020510745</v>
+        <v>0.1274223660873257</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.0559647366176912</v>
+        <v>0.1436516216587599</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.09227048700386169</v>
+        <v>0.154652544849109</v>
       </c>
       <c r="AF11" t="n">
-        <v>9.590738484617166</v>
+        <v>6.321034377004751</v>
       </c>
       <c r="AG11" t="n">
-        <v>17.1164373196421</v>
+        <v>8.368214793983025</v>
       </c>
       <c r="AH11" t="n">
-        <v>27.38228133952566</v>
+        <v>11.09766570508671</v>
       </c>
       <c r="AI11" t="n">
-        <v>29.80101385244161</v>
+        <v>14.16143644665081</v>
       </c>
       <c r="AJ11" t="n">
-        <v>43.13399308197712</v>
+        <v>17.79169696120602</v>
       </c>
       <c r="AK11" t="n">
-        <v>4.792434012937949</v>
+        <v>2.005865714157519</v>
       </c>
       <c r="AL11" t="n">
-        <v>6.32345605572704</v>
+        <v>2.444539278320115</v>
       </c>
       <c r="AM11" t="n">
-        <v>7.048181356039972</v>
+        <v>2.731027709969486</v>
       </c>
       <c r="AN11" t="n">
-        <v>8.272907588699205</v>
+        <v>3.490291318965492</v>
       </c>
       <c r="AO11" t="n">
-        <v>10.61449378587335</v>
+        <v>4.42726365946269</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
+          <t>ngB_general</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>45.93343593776623</v>
+      </c>
+      <c r="C12" t="n">
+        <v>45.93343593776623</v>
+      </c>
+      <c r="D12" t="n">
+        <v>45.93343593776623</v>
+      </c>
+      <c r="E12" t="n">
+        <v>45.93343593776623</v>
+      </c>
+      <c r="F12" t="n">
+        <v>45.93343593776623</v>
+      </c>
+      <c r="G12" t="n">
+        <v>27.8335508740337</v>
+      </c>
+      <c r="H12" t="n">
+        <v>27.8335508740337</v>
+      </c>
+      <c r="I12" t="n">
+        <v>27.8335508740337</v>
+      </c>
+      <c r="J12" t="n">
+        <v>27.8335508740337</v>
+      </c>
+      <c r="K12" t="n">
+        <v>27.8335508740337</v>
+      </c>
+      <c r="L12" t="n">
+        <v>10.90561836300458</v>
+      </c>
+      <c r="M12" t="n">
+        <v>10.90561836300458</v>
+      </c>
+      <c r="N12" t="n">
+        <v>10.90561836300458</v>
+      </c>
+      <c r="O12" t="n">
+        <v>10.90561836300458</v>
+      </c>
+      <c r="P12" t="n">
+        <v>10.90561836300458</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>32.34287855581071</v>
+      </c>
+      <c r="R12" t="n">
+        <v>37.12596960377323</v>
+      </c>
+      <c r="S12" t="n">
+        <v>41.4346808128283</v>
+      </c>
+      <c r="T12" t="n">
+        <v>45.89228111450264</v>
+      </c>
+      <c r="U12" t="n">
+        <v>56.29327659719353</v>
+      </c>
+      <c r="V12" t="n">
+        <v>61.07248296316209</v>
+      </c>
+      <c r="W12" t="n">
+        <v>68.08291448987606</v>
+      </c>
+      <c r="X12" t="n">
+        <v>75.28289368015302</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>81.12896259701462</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>92.93364477701869</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.1093813318630674</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.1218133951515619</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.1336203819946245</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.1466853145489766</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.1634946895006716</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>6.23955616941171</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>8.622953930919012</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>11.71548158223406</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>14.55382326654365</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>16.887125861169</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>2.029222237034199</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>2.370941285477072</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>2.917603187897584</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>3.633613868001115</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>4.550336077016741</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>reB_BeijingChina</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="C13" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="D13" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="E13" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="F13" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="G13" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="H13" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="I13" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="J13" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="K13" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="L13" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="M13" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="N13" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="O13" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="P13" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>45.9755801865513</v>
+      </c>
+      <c r="R13" t="n">
+        <v>51.95391108225861</v>
+      </c>
+      <c r="S13" t="n">
+        <v>58.90375450110832</v>
+      </c>
+      <c r="T13" t="n">
+        <v>68.58739953646852</v>
+      </c>
+      <c r="U13" t="n">
+        <v>82.79488837825491</v>
+      </c>
+      <c r="V13" t="n">
+        <v>109.0701452981848</v>
+      </c>
+      <c r="W13" t="n">
+        <v>135.2275623820017</v>
+      </c>
+      <c r="X13" t="n">
+        <v>156.5114130391525</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>174.8085923611451</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>209.7276801977513</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>-0.1100363334788378</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>-0.03594897666949413</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.02389131038891967</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.09895754078020513</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.1598633678087175</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>9.935854857773078</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>17.77741037569217</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>25.62826112272937</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>33.49728232452985</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>47.10255516741271</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0.8935737359571084</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>1.835580145782627</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>2.830406254263417</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>3.868765442301612</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>5.675436251157488</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>reB_general</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="C14" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="D14" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="E14" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="F14" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="G14" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="H14" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="I14" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="J14" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="K14" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="L14" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="M14" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="N14" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="O14" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="P14" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>44.54177192662276</v>
+      </c>
+      <c r="R14" t="n">
+        <v>50.08533733706039</v>
+      </c>
+      <c r="S14" t="n">
+        <v>60.81717720760438</v>
+      </c>
+      <c r="T14" t="n">
+        <v>71.07758666298615</v>
+      </c>
+      <c r="U14" t="n">
+        <v>81.51712295675212</v>
+      </c>
+      <c r="V14" t="n">
+        <v>109.4336159230961</v>
+      </c>
+      <c r="W14" t="n">
+        <v>127.4175143665883</v>
+      </c>
+      <c r="X14" t="n">
+        <v>151.2273989981154</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>172.1212580167213</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>198.631151978875</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>-0.1239557458932592</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>-0.01552585102099389</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0.05358286744075112</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.09452753607670755</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.1518977710013762</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>11.37818752047522</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>15.45442735375627</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>25.31299509223773</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>36.30786513896947</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>46.49557475318914</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>0.4819708150770097</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>1.959848720400444</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>2.988644107923881</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>4.028798525975993</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>5.64406499554128</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>reC_BeijingChina</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="C15" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="D15" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="E15" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="F15" t="n">
+        <v>71.44512899511798</v>
+      </c>
+      <c r="G15" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="H15" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="I15" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="J15" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="K15" t="n">
+        <v>91.79485817690723</v>
+      </c>
+      <c r="L15" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="M15" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="N15" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="O15" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="P15" t="n">
+        <v>17.94858176907224</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>50.74495988965502</v>
+      </c>
+      <c r="R15" t="n">
+        <v>57.44583060962253</v>
+      </c>
+      <c r="S15" t="n">
+        <v>64.36924092913125</v>
+      </c>
+      <c r="T15" t="n">
+        <v>74.05557755758502</v>
+      </c>
+      <c r="U15" t="n">
+        <v>87.5344095139795</v>
+      </c>
+      <c r="V15" t="n">
+        <v>65.80805301830486</v>
+      </c>
+      <c r="W15" t="n">
+        <v>93.90822569245803</v>
+      </c>
+      <c r="X15" t="n">
+        <v>113.4856955659664</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>132.8240894627759</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>170.6650944424859</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>-0.2246777328552557</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>-0.1637511664321824</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>-0.1092182855299161</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>-0.03444798303089411</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.01934772459668259</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>7.856185552376402</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>15.59078273145933</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>23.40078898799183</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>31.82040803703839</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>44.56569767442517</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>-0.5457116357409506</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>0.4667399534667621</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>1.318652746697537</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>2.292803992612368</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>4.084146992614196</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
           <t>reC_general</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B16" t="n">
         <v>71.44512899511798</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C16" t="n">
         <v>71.44512899511798</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D16" t="n">
         <v>71.44512899511798</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E16" t="n">
         <v>71.44512899511798</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F16" t="n">
         <v>71.44512899511798</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G16" t="n">
         <v>91.79485817690723</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H16" t="n">
         <v>91.79485817690723</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I16" t="n">
         <v>91.79485817690723</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J16" t="n">
         <v>91.79485817690723</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K16" t="n">
         <v>91.79485817690723</v>
       </c>
-      <c r="L12" t="n">
+      <c r="L16" t="n">
         <v>17.94858176907224</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M16" t="n">
         <v>17.94858176907224</v>
       </c>
-      <c r="N12" t="n">
+      <c r="N16" t="n">
         <v>17.94858176907224</v>
       </c>
-      <c r="O12" t="n">
+      <c r="O16" t="n">
         <v>17.94858176907224</v>
       </c>
-      <c r="P12" t="n">
+      <c r="P16" t="n">
         <v>17.94858176907224</v>
       </c>
-      <c r="Q12" t="n">
-        <v>92.92089423699838</v>
-      </c>
-      <c r="R12" t="n">
-        <v>99.26410196145389</v>
-      </c>
-      <c r="S12" t="n">
-        <v>117.0401922191223</v>
-      </c>
-      <c r="T12" t="n">
-        <v>147.5949304038306</v>
-      </c>
-      <c r="U12" t="n">
-        <v>167.5147632932046</v>
-      </c>
-      <c r="V12" t="n">
-        <v>71.66555075784566</v>
-      </c>
-      <c r="W12" t="n">
-        <v>95.51685702066928</v>
-      </c>
-      <c r="X12" t="n">
-        <v>139.4837885833368</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>152.6534511650603</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>176.6591994064799</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>-0.1163842576664746</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>-0.06873232053977801</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>-0.02916979650479175</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>0.005859606878129458</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>0.1210975373427857</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>9.901647850780995</v>
-      </c>
-      <c r="AG12" t="n">
-        <v>15.26923420138435</v>
-      </c>
-      <c r="AH12" t="n">
-        <v>22.68750362838114</v>
-      </c>
-      <c r="AI12" t="n">
-        <v>37.35915287550591</v>
-      </c>
-      <c r="AJ12" t="n">
-        <v>42.7364958508017</v>
-      </c>
-      <c r="AK12" t="n">
-        <v>4.077168408607911</v>
-      </c>
-      <c r="AL12" t="n">
-        <v>5.26263230634667</v>
-      </c>
-      <c r="AM12" t="n">
-        <v>7.216262127936014</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>9.382017865577062</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>10.71195600932494</v>
+      <c r="Q16" t="n">
+        <v>50.0275178621409</v>
+      </c>
+      <c r="R16" t="n">
+        <v>55.83089057061396</v>
+      </c>
+      <c r="S16" t="n">
+        <v>65.88774944874996</v>
+      </c>
+      <c r="T16" t="n">
+        <v>75.8852748135436</v>
+      </c>
+      <c r="U16" t="n">
+        <v>86.13969442910116</v>
+      </c>
+      <c r="V16" t="n">
+        <v>71.2460652079732</v>
+      </c>
+      <c r="W16" t="n">
+        <v>89.63800139325227</v>
+      </c>
+      <c r="X16" t="n">
+        <v>112.6677346381996</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>135.2117280749629</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>158.7348551904529</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>-0.2536021708941236</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>-0.1605451719378048</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>-0.09525384118353758</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>-0.04352071921642764</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0.0077746002440057</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>9.022167587574188</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>13.3957244849251</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>23.15742746045262</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>34.24286233462494</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>43.91437916327281</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>-1.129959917641097</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>0.4719081383276267</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>1.468488617995145</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>2.486823314275663</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>3.984867859014028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>